<commit_message>
sprites voor super star wars klaar
</commit_message>
<xml_diff>
--- a/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
+++ b/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2019_2020\_Programming2\00_GameProject\ForStudents\Description&amp;Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarne\Documents\DAE\sem_2\programming_2\Wieme_Jarne_SuperStarWars\Wieme_Jarne_SuperStarWars\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4984F497-55EC-4B83-ADE3-1FA07A0C4370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="975" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Game rubric" sheetId="2" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Camera</t>
   </si>
@@ -101,11 +102,14 @@
   <si>
     <t>Animation system based on data from a file</t>
   </si>
+  <si>
+    <t>klaar op 09/03/'22</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,8 +217,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Kop 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -496,96 +500,220 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="74" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="80.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.21875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="80.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -593,130 +721,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="57.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="74" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m99485b88215436a82099f8287cba0b0>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100723942CCEB3A674D8F1F6472CCEFB38E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b456a193ed59fb7b1c8994f62cf0bc67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xmlns:ns3="60eb0cf4-ae2a-4762-800a-cb593b869ecb" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="a2e691a9-fcfc-4d85-a390-1894fe98bd9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a253e5da7d9e3ac9660eca9ce8fbd104" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
@@ -969,35 +995,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m99485b88215436a82099f8287cba0b0>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}"/>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <ds:schemaRef ds:uri="60eb0cf4-ae2a-4762-800a-cb593b869ecb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="a2e691a9-fcfc-4d85-a390-1894fe98bd9e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
mario ass game design ingediend en gewerkt aan super star wars
</commit_message>
<xml_diff>
--- a/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
+++ b/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarne\Documents\DAE\sem_2\programming_2\Wieme_Jarne_SuperStarWars\Wieme_Jarne_SuperStarWars\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4984F497-55EC-4B83-ADE3-1FA07A0C4370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7954521A-B778-46BB-BCCB-0DB4EEB7416F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="975" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Camera</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>klaar op 09/03/'22</t>
+  </si>
+  <si>
+    <t>klaar op 12/03/'22</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +536,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -606,7 +612,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +654,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -722,27 +728,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m99485b88215436a82099f8287cba0b0>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100723942CCEB3A674D8F1F6472CCEFB38E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b456a193ed59fb7b1c8994f62cf0bc67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xmlns:ns3="60eb0cf4-ae2a-4762-800a-cb593b869ecb" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="a2e691a9-fcfc-4d85-a390-1894fe98bd9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a253e5da7d9e3ac9660eca9ce8fbd104" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
@@ -995,26 +980,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m99485b88215436a82099f8287cba0b0>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1033,4 +1020,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
sliding toegevoegd en schieten werkt bijne goed
</commit_message>
<xml_diff>
--- a/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
+++ b/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarne\Documents\DAE\sem_2\programming_2\Wieme_Jarne_SuperStarWars\Wieme_Jarne_SuperStarWars\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7954521A-B778-46BB-BCCB-0DB4EEB7416F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1018F6-EE07-4187-9085-A92F08434968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="975" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Camera</t>
   </si>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>Animation system based on data from a file</t>
-  </si>
-  <si>
-    <t>klaar op 09/03/'22</t>
-  </si>
-  <si>
-    <t>klaar op 12/03/'22</t>
   </si>
 </sst>
 </file>
@@ -510,7 +504,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,10 +530,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -547,10 +538,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -728,6 +716,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m99485b88215436a82099f8287cba0b0>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100723942CCEB3A674D8F1F6472CCEFB38E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b456a193ed59fb7b1c8994f62cf0bc67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xmlns:ns3="60eb0cf4-ae2a-4762-800a-cb593b869ecb" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="a2e691a9-fcfc-4d85-a390-1894fe98bd9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a253e5da7d9e3ac9660eca9ce8fbd104" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
@@ -980,28 +989,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m99485b88215436a82099f8287cba0b0>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1020,23 +1027,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
powerup en jumpingEnemy toegevoegd aan super star wars
</commit_message>
<xml_diff>
--- a/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
+++ b/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarne\Documents\DAE\sem_2\programming_2\Wieme_Jarne_SuperStarWars\Wieme_Jarne_SuperStarWars\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarne\Documents\DAE\sem_2\programming_2\Wieme_Jarne_SuperStarWars\Wieme_Jarne_SuperStarWars\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1018F6-EE07-4187-9085-A92F08434968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC127FEC-8B19-4C87-8F16-5AD4F1210209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="975" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Game rubric" sheetId="2" r:id="rId1"/>
@@ -504,7 +504,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -555,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -716,27 +716,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m99485b88215436a82099f8287cba0b0>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100723942CCEB3A674D8F1F6472CCEFB38E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b456a193ed59fb7b1c8994f62cf0bc67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xmlns:ns3="60eb0cf4-ae2a-4762-800a-cb593b869ecb" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="a2e691a9-fcfc-4d85-a390-1894fe98bd9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a253e5da7d9e3ac9660eca9ce8fbd104" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
@@ -989,26 +968,28 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m99485b88215436a82099f8287cba0b0>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1027,4 +1008,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
grading rubric bekeken en nog een paar dingen aangepast aan super star wars
</commit_message>
<xml_diff>
--- a/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
+++ b/sem_2/programming_2/Wieme_Jarne_SuperStarWars/Wieme_Jarne_SuperStarWars/Resources/Wieme_Jarne_SuperStarWars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarne\Documents\DAE\sem_2\programming_2\Wieme_Jarne_SuperStarWars\Wieme_Jarne_SuperStarWars\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC127FEC-8B19-4C87-8F16-5AD4F1210209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F82E4D-E2B7-4F10-A2EE-125E769460FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,7 +504,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -716,6 +716,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m99485b88215436a82099f8287cba0b0>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100723942CCEB3A674D8F1F6472CCEFB38E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b456a193ed59fb7b1c8994f62cf0bc67">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="128482ec-0431-40d5-ab26-89ea2a4f3ccd" xmlns:ns3="60eb0cf4-ae2a-4762-800a-cb593b869ecb" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns5="a2e691a9-fcfc-4d85-a390-1894fe98bd9e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a253e5da7d9e3ac9660eca9ce8fbd104" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
     <xsd:import namespace="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
@@ -968,28 +989,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <TaxCatchAll xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-    <m99485b88215436a82099f8287cba0b0 xmlns="128482ec-0431-40d5-ab26-89ea2a4f3ccd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m99485b88215436a82099f8287cba0b0>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBBEFD80-C66F-4B0C-9ED1-734A448E3DFF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1008,23 +1027,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E48979D-1BFD-4ABF-A49B-E2BDAD7A21BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B0CCE84-996D-4970-9B0F-6A269E60B9CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="128482ec-0431-40d5-ab26-89ea2a4f3ccd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>